<commit_message>
udpated getting started info
</commit_message>
<xml_diff>
--- a/hosted_files/dataset.xlsx
+++ b/hosted_files/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peli/Documents/data-science-editor-excel/hosted_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA50ED9B-ED7B-F345-ABFC-B085E8ED4329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CB9E92-0A32-5E46-ACD3-021626A81BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="287">
   <si>
     <t>name</t>
   </si>
@@ -3639,6 +3639,12 @@
       </rPr>
       <t>is available from then Office Store at</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://microsoft.github.io/data-science-editor-excel/hosted_files/getting-started.gif </t>
+  </si>
+  <si>
+    <t>This video shows the basic usage of the Data Science Editor addin.</t>
   </si>
 </sst>
 </file>
@@ -5434,6 +5440,151 @@
               <a:cs typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>add-in</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2488958</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>5096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="LaunchHelpHeader">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECAC3A8-B524-D844-9294-3C9E85AEB63A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="368301" y="6515100"/>
+          <a:ext cx="10934457" cy="513096"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="0" rtlCol="0" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400">
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Getting started</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8267,7 +8418,7 @@
   <dimension ref="B1:D28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8341,17 +8492,21 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="6"/>
+    <row r="20" spans="2:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="B20" s="34" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
+    <row r="22" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="6"/>
@@ -8374,10 +8529,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{77612E16-80A7-B340-B4E4-838CBA0512B6}"/>
+    <hyperlink ref="B22" r:id="rId2" xr:uid="{CE2008CE-EA29-FF43-BACC-29E9296E5E61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>